<commit_message>
Estabilización de pagos en Android
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/pagos/TarjetaCreditoNoPropia.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/pagos/TarjetaCreditoNoPropia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\Daniel Torres Devco\todo1\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\pagos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F402B8-82E0-410C-80E9-6D1771BC7799}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78EF2A4-BFB9-4B9E-BC19-591F45393AA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="51">
   <si>
     <t>ID</t>
   </si>
@@ -121,9 +121,6 @@
     <t>valorPago</t>
   </si>
   <si>
-    <t>4444444444444444</t>
-  </si>
-  <si>
     <t>Pago mínimo en pesos</t>
   </si>
   <si>
@@ -142,21 +139,12 @@
     <t>Otro valor</t>
   </si>
   <si>
-    <t>120000</t>
-  </si>
-  <si>
     <t>Dólares</t>
   </si>
   <si>
-    <t>5326666666666666</t>
-  </si>
-  <si>
     <t>Pago total en dólares</t>
   </si>
   <si>
-    <t>80000</t>
-  </si>
-  <si>
     <t>22493944</t>
   </si>
   <si>
@@ -170,6 +158,21 @@
   </si>
   <si>
     <t>406-725170-07</t>
+  </si>
+  <si>
+    <t>5303710149825215</t>
+  </si>
+  <si>
+    <t>4513070436920974</t>
+  </si>
+  <si>
+    <t>5303710095505365</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>1200</t>
   </si>
 </sst>
 </file>
@@ -606,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -678,7 +681,7 @@
         <v>32</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>25</v>
@@ -692,13 +695,13 @@
         <v>14</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>23</v>
@@ -731,22 +734,22 @@
         <v>22</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q2" s="10" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="R2" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S2" s="10" t="s">
         <v>29</v>
       </c>
       <c r="T2" s="13" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="10" customFormat="1">
@@ -754,13 +757,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>23</v>
@@ -793,22 +796,22 @@
         <v>22</v>
       </c>
       <c r="O3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="Q3" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="R3" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="Q3" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="R3" s="10" t="s">
-        <v>41</v>
-      </c>
       <c r="S3" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="T3" s="13" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -816,13 +819,13 @@
         <v>27</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>23</v>
@@ -855,22 +858,22 @@
         <v>22</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="Q4" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R4" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="S4" s="10" t="s">
         <v>29</v>
       </c>
       <c r="T4" s="13" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -878,13 +881,13 @@
         <v>28</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>23</v>
@@ -917,22 +920,22 @@
         <v>22</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="P5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q5" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="Q5" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="R5" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S5" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="T5" s="13" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>